<commit_message>
Added Pylint and Pytest
</commit_message>
<xml_diff>
--- a/3_Implementation/src/NewData.xlsx
+++ b/3_Implementation/src/NewData.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:U6"/>
@@ -2075,6 +2075,1026 @@
         </is>
       </c>
       <c r="U16" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PS Number</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hindi</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Biology</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Physics</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Telugu</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>C-Programming</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Processor and Controllers</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Analog Communication</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Digital Communication</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Operating systems</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Web Technologies</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Engineering Drawing</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Geography</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Civics </t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>99004400</v>
+      </c>
+      <c r="B18" t="n">
+        <v>95</v>
+      </c>
+      <c r="C18" t="n">
+        <v>98</v>
+      </c>
+      <c r="D18" t="n">
+        <v>87</v>
+      </c>
+      <c r="E18" t="n">
+        <v>79</v>
+      </c>
+      <c r="F18" t="n">
+        <v>65</v>
+      </c>
+      <c r="G18" t="n">
+        <v>90</v>
+      </c>
+      <c r="H18" t="n">
+        <v>87</v>
+      </c>
+      <c r="I18" t="n">
+        <v>95</v>
+      </c>
+      <c r="J18" t="n">
+        <v>74</v>
+      </c>
+      <c r="K18" t="n">
+        <v>86</v>
+      </c>
+      <c r="L18" t="n">
+        <v>75</v>
+      </c>
+      <c r="M18" t="n">
+        <v>88</v>
+      </c>
+      <c r="N18" t="n">
+        <v>76</v>
+      </c>
+      <c r="O18" t="n">
+        <v>87</v>
+      </c>
+      <c r="P18" t="n">
+        <v>66</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>79</v>
+      </c>
+      <c r="R18" t="n">
+        <v>80</v>
+      </c>
+      <c r="S18" t="n">
+        <v>82</v>
+      </c>
+      <c r="T18" t="n">
+        <v>76</v>
+      </c>
+      <c r="U18" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PS Number</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Hobby 1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hobby 2</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Hobby 3</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Hobby 4</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Hobby 5</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Hobby 6</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Hobby 7</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Hobby 8</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Hobby 9</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Hobby 10</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Hobby 11</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Hobby 12</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Hobby 13</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Hobby 14</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Hobby 15</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Hobby 16</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Hobby 17</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Hobby 18</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Hobby 19</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Hobby 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>99004408</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Go Camping</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Watch Documentaries</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>New Music Discovery</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Computer Programming</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Fishing</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Walking</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Travelling</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Golf</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Exercise</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Drawing</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Sewing</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Hiking</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Cooking</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Scrapbooking</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Cross-Stitch</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Jigsaw puzzel</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Parachuting</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Genealogy</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Computer Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PS Number</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>City 1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> City 2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> City 3</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>City 4</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>City 5</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>City 6</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>City 7</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>City 8</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>City 9</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>City 10</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>City 11</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>City 12</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>City 13</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>City 14</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>City 15</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>City 16</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>City 17</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>City 18</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>City 19</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>City 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>99004412</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Gwalior</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Noida</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Jamshedpur</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Cuttak</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ajmer</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Jammu</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Tirupathi</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Kakinada</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Khammam</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Nizamabad</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Thiruvananthapur</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Guwahati</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Meerut</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Raipur</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Shimla</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Jodhpur</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Ujjain</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Udhaipur</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Gandhinagar</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PS Number</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Java Script</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Go</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Perl</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ruby</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Swift</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Scala</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>PHP</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>SQL</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Arduino</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Matlab</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Rust</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Type Script</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Kotlin</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>CSS</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Powershell</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>99004402</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Competent</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Competent</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Competent</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Competent</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Proficient</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PS Number</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Sport 1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Sport 2</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Sport 3</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Sport 4</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Sport 5</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Sport 6</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Sport 7</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Sport 8</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sport 9 </t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Sport 10</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Sport 11</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Sport 12</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Sport 13</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Sport 14</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Sport 15</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Sport 16</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Sport 17</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Sport 18</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Sport 19</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Sport 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>99004402</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bungee Jumping</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Hockey</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Car Racing</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Cricket</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Chess</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Carroms</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Dodgeball</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Darts</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Handball</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Hockey</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Kendo</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Squash</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Softball</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Soccer</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Tennis</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Baseball</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Golf</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
         <is>
           <t>Running</t>
         </is>

</xml_diff>